<commit_message>
Update src code for CARLA dataset generation. Update CARLA datset spec for latest dataset images - 06032020
</commit_message>
<xml_diff>
--- a/carla_dataset_spec.xlsx
+++ b/carla_dataset_spec.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Projects\TRIP_endtoend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC9ECA6-EB76-415D-B7A1-D2B4F69645F5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62CDA3C-075E-4194-A859-231664BABB6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16716" yWindow="3876" windowWidth="12600" windowHeight="10404" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specifications" sheetId="1" r:id="rId1"/>
-    <sheet name="Information" sheetId="2" r:id="rId2"/>
+    <sheet name="Dataset_info" sheetId="5" r:id="rId2"/>
+    <sheet name="Information" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="45">
   <si>
     <t xml:space="preserve">Number of location </t>
   </si>
@@ -116,6 +117,57 @@
   </si>
   <si>
     <t>Car vs Pedestrians</t>
+  </si>
+  <si>
+    <t>Phases</t>
+  </si>
+  <si>
+    <t>No of images</t>
+  </si>
+  <si>
+    <t>Town_01</t>
+  </si>
+  <si>
+    <t>Town_02</t>
+  </si>
+  <si>
+    <t>Town_03</t>
+  </si>
+  <si>
+    <t>Town_04</t>
+  </si>
+  <si>
+    <t>Town_05</t>
+  </si>
+  <si>
+    <t>Town_06</t>
+  </si>
+  <si>
+    <t>Town_07</t>
+  </si>
+  <si>
+    <t>Phase 1</t>
+  </si>
+  <si>
+    <t>Phase 2</t>
+  </si>
+  <si>
+    <t>Phase 3</t>
+  </si>
+  <si>
+    <t>Phase 4</t>
+  </si>
+  <si>
+    <t>Phase 5</t>
+  </si>
+  <si>
+    <t>Phase 6</t>
+  </si>
+  <si>
+    <t>Phase 7</t>
+  </si>
+  <si>
+    <t>Total images</t>
   </si>
 </sst>
 </file>
@@ -145,7 +197,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -168,18 +220,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,7 +565,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -539,10 +640,326 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00274F18-CD51-4890-BCCF-C34AA83C50A5}">
+  <dimension ref="A1:C33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
+      <c r="B24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
+      <c r="B26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
+      <c r="B28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2"/>
+      <c r="B32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" s="1">
+        <f>SUM(C2:C32)</f>
+        <v>3070</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A18:A22"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE77FD5B-5F6C-43BD-9C48-E6E44D09D4F3}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B11" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
@@ -572,7 +989,7 @@
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -582,7 +999,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
@@ -590,7 +1007,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
@@ -678,7 +1095,7 @@
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -688,7 +1105,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
+      <c r="B15" s="4"/>
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
@@ -696,7 +1113,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
+      <c r="B16" s="4"/>
       <c r="C16" s="1" t="s">
         <v>27</v>
       </c>
@@ -784,7 +1201,7 @@
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -794,7 +1211,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
+      <c r="B27" s="4"/>
       <c r="C27" s="1" t="s">
         <v>26</v>
       </c>
@@ -802,7 +1219,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
+      <c r="B28" s="4"/>
       <c r="C28" s="1" t="s">
         <v>27</v>
       </c>
@@ -890,7 +1307,7 @@
       <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -900,7 +1317,7 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
-      <c r="B39" s="3"/>
+      <c r="B39" s="4"/>
       <c r="C39" s="1" t="s">
         <v>26</v>
       </c>
@@ -908,7 +1325,7 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
-      <c r="B40" s="3"/>
+      <c r="B40" s="4"/>
       <c r="C40" s="1" t="s">
         <v>27</v>
       </c>
@@ -1022,7 +1439,7 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -1032,7 +1449,7 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
-      <c r="B54" s="3"/>
+      <c r="B54" s="4"/>
       <c r="C54" s="1" t="s">
         <v>26</v>
       </c>
@@ -1040,7 +1457,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
-      <c r="B55" s="3"/>
+      <c r="B55" s="4"/>
       <c r="C55" s="1" t="s">
         <v>27</v>
       </c>
@@ -1126,11 +1543,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="A50:A64"/>
     <mergeCell ref="B35:B37"/>
@@ -1146,12 +1563,12 @@
     <mergeCell ref="B26:B28"/>
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B32:B34"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
     <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="B62:B64"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New batch file for running CARLA evaluation src code (carla_trip_evaluate.bat). Separate NPC spawning into a new function (carla_trip_evaluation_2.py). Update dataset_spec - 06052020
</commit_message>
<xml_diff>
--- a/carla_dataset_spec.xlsx
+++ b/carla_dataset_spec.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Projects\TRIP_endtoend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atsumilab\Documents\Projects\TRIP_endtoend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62CDA3C-075E-4194-A859-231664BABB6F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16716" yWindow="3876" windowWidth="12600" windowHeight="10404" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16710" yWindow="3870" windowWidth="12600" windowHeight="10410" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Specifications" sheetId="1" r:id="rId1"/>
     <sheet name="Dataset_info" sheetId="5" r:id="rId2"/>
     <sheet name="Information" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="48">
   <si>
     <t xml:space="preserve">Number of location </t>
   </si>
@@ -168,12 +167,21 @@
   </si>
   <si>
     <t>Total images</t>
+  </si>
+  <si>
+    <t>Phase 8</t>
+  </si>
+  <si>
+    <t>Phase 9</t>
+  </si>
+  <si>
+    <t>Phase 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -261,17 +269,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -282,9 +284,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -561,21 +575,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,7 +597,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -591,7 +605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -599,7 +613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -607,7 +621,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -618,7 +632,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -626,7 +640,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -640,20 +654,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00274F18-CD51-4890-BCCF-C34AA83C50A5}">
-  <dimension ref="A1:C33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -664,8 +678,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -675,17 +689,17 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>39</v>
       </c>
@@ -693,8 +707,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>40</v>
       </c>
@@ -702,17 +716,17 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>42</v>
       </c>
@@ -720,235 +734,339 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1" t="s">
+      <c r="C10" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1" t="s">
+      <c r="C11" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="C12" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+      <c r="B14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="1" t="s">
+      <c r="C16" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1" t="s">
+      <c r="C17" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1" t="s">
+      <c r="C18" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="1" t="s">
+      <c r="C19" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="1" t="s">
+      <c r="C20" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="1">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C21" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="B28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="C30" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4"/>
+      <c r="B31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="1" t="s">
+      <c r="C33" s="1">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="1"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="1" t="s">
+      <c r="C34" s="1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="1"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="1" t="s">
+      <c r="C35" s="1">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C27" s="1"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
-      <c r="B28" s="1" t="s">
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="1"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="1" t="s">
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="B31" s="1" t="s">
+      <c r="C40" s="1"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="1" t="s">
+      <c r="C41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
+      <c r="B42" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="1">
-        <f>SUM(C2:C32)</f>
-        <v>3070</v>
+      <c r="B43" s="2"/>
+      <c r="C43" s="1">
+        <f>SUM(C2:C42)</f>
+        <v>7000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A40:A42"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A10:A15"/>
+    <mergeCell ref="A16:A25"/>
+    <mergeCell ref="A26:A32"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -956,22 +1074,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE77FD5B-5F6C-43BD-9C48-E6E44D09D4F3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B11" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -985,11 +1103,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -997,23 +1115,23 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="4"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="4"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>22</v>
@@ -1023,7 +1141,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
@@ -1031,7 +1149,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
@@ -1039,7 +1157,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>23</v>
@@ -1049,7 +1167,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
@@ -1057,7 +1175,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
@@ -1065,7 +1183,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>24</v>
@@ -1075,7 +1193,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1" t="s">
@@ -1083,7 +1201,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
@@ -1091,11 +1209,11 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -1103,23 +1221,23 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="4"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="4"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>22</v>
@@ -1129,7 +1247,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
@@ -1137,7 +1255,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
@@ -1145,7 +1263,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
         <v>23</v>
@@ -1155,7 +1273,7 @@
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
@@ -1163,7 +1281,7 @@
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1" t="s">
@@ -1171,7 +1289,7 @@
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
         <v>24</v>
@@ -1181,7 +1299,7 @@
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="1" t="s">
@@ -1189,7 +1307,7 @@
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="1" t="s">
@@ -1197,11 +1315,11 @@
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1209,23 +1327,23 @@
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="4"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="4"/>
+      <c r="B28" s="9"/>
       <c r="C28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
         <v>22</v>
@@ -1235,7 +1353,7 @@
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="1" t="s">
@@ -1243,7 +1361,7 @@
       </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="1" t="s">
@@ -1251,7 +1369,7 @@
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
         <v>23</v>
@@ -1261,7 +1379,7 @@
       </c>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="1" t="s">
@@ -1269,7 +1387,7 @@
       </c>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="1" t="s">
@@ -1277,7 +1395,7 @@
       </c>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
         <v>24</v>
@@ -1287,7 +1405,7 @@
       </c>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="1" t="s">
@@ -1295,7 +1413,7 @@
       </c>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="1" t="s">
@@ -1303,11 +1421,11 @@
       </c>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1315,23 +1433,23 @@
       </c>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
-      <c r="B39" s="4"/>
+      <c r="B39" s="9"/>
       <c r="C39" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="B40" s="4"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
         <v>22</v>
@@ -1341,7 +1459,7 @@
       </c>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="1" t="s">
@@ -1349,7 +1467,7 @@
       </c>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="1" t="s">
@@ -1357,7 +1475,7 @@
       </c>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
         <v>23</v>
@@ -1367,7 +1485,7 @@
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="1" t="s">
@@ -1375,7 +1493,7 @@
       </c>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="1" t="s">
@@ -1383,7 +1501,7 @@
       </c>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
         <v>24</v>
@@ -1393,7 +1511,7 @@
       </c>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="1" t="s">
@@ -1401,7 +1519,7 @@
       </c>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="1" t="s">
@@ -1409,7 +1527,7 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>17</v>
       </c>
@@ -1421,7 +1539,7 @@
       </c>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="1" t="s">
@@ -1429,7 +1547,7 @@
       </c>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="1" t="s">
@@ -1437,9 +1555,9 @@
       </c>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -1447,23 +1565,23 @@
       </c>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
-      <c r="B54" s="4"/>
+      <c r="B54" s="9"/>
       <c r="C54" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
-      <c r="B55" s="4"/>
+      <c r="B55" s="9"/>
       <c r="C55" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
         <v>22</v>
@@ -1473,7 +1591,7 @@
       </c>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="1" t="s">
@@ -1481,7 +1599,7 @@
       </c>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="1" t="s">
@@ -1489,7 +1607,7 @@
       </c>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2" t="s">
         <v>23</v>
@@ -1499,7 +1617,7 @@
       </c>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="1" t="s">
@@ -1507,7 +1625,7 @@
       </c>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="1" t="s">
@@ -1515,7 +1633,7 @@
       </c>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
         <v>24</v>
@@ -1525,7 +1643,7 @@
       </c>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="1" t="s">
@@ -1533,7 +1651,7 @@
       </c>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="1" t="s">

</xml_diff>

<commit_message>
Update src code and spec file - 06072020
</commit_message>
<xml_diff>
--- a/carla_dataset_spec.xlsx
+++ b/carla_dataset_spec.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="48">
   <si>
     <t xml:space="preserve">Number of location </t>
   </si>
@@ -655,16 +655,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -966,107 +966,205 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C33" s="1">
-        <v>1800</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
+      <c r="A34" s="4"/>
       <c r="B34" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C34" s="1">
-        <v>700</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
+      <c r="A35" s="4"/>
       <c r="B35" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="1">
-        <v>1400</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
+      <c r="A36" s="4"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="1"/>
+      <c r="C36" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="4"/>
+      <c r="B37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="1"/>
+      <c r="C40" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
+      <c r="A41" s="4"/>
       <c r="B41" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="1"/>
+      <c r="C41" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
+      <c r="A42" s="4"/>
       <c r="B42" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="1"/>
+      <c r="C42" s="1">
+        <v>100</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="4"/>
+      <c r="B43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="B47" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="1">
-        <f>SUM(C2:C42)</f>
-        <v>7000</v>
+      <c r="B53" s="2"/>
+      <c r="C53" s="1">
+        <f>SUM(C2:C52)</f>
+        <v>4800</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A40:A42"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A50:A52"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="A10:A15"/>
     <mergeCell ref="A16:A25"/>
     <mergeCell ref="A26:A32"/>
+    <mergeCell ref="A33:A39"/>
+    <mergeCell ref="A40:A49"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update dataset size for CARLA virtual image - 06172020
</commit_message>
<xml_diff>
--- a/carla_dataset_spec.xlsx
+++ b/carla_dataset_spec.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atsumilab\Documents\Projects\TRIP_endtoend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Projects\TRIP_endtoend\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DBA56F-E665-4C7A-9498-872F6A74BD92}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16710" yWindow="3870" windowWidth="12600" windowHeight="10410" activeTab="1"/>
+    <workbookView xWindow="10440" yWindow="1956" windowWidth="12600" windowHeight="10404" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specifications" sheetId="1" r:id="rId1"/>
     <sheet name="Dataset_info" sheetId="5" r:id="rId2"/>
     <sheet name="Information" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="65">
   <si>
     <t xml:space="preserve">Number of location </t>
   </si>
@@ -176,12 +177,63 @@
   </si>
   <si>
     <t>Phase 10</t>
+  </si>
+  <si>
+    <t>Phase 11</t>
+  </si>
+  <si>
+    <t>Phase 12</t>
+  </si>
+  <si>
+    <t>Phase 13</t>
+  </si>
+  <si>
+    <t>Phase 14</t>
+  </si>
+  <si>
+    <t>Phase 15</t>
+  </si>
+  <si>
+    <t>Phase 16</t>
+  </si>
+  <si>
+    <t>Phase 17</t>
+  </si>
+  <si>
+    <t>Phase 18</t>
+  </si>
+  <si>
+    <t>Phase 19</t>
+  </si>
+  <si>
+    <t>Phase 20</t>
+  </si>
+  <si>
+    <t>Phase 21</t>
+  </si>
+  <si>
+    <t>Phase 22</t>
+  </si>
+  <si>
+    <t>Phase 23</t>
+  </si>
+  <si>
+    <t>Phase 24</t>
+  </si>
+  <si>
+    <t>Phase 25</t>
+  </si>
+  <si>
+    <t>Phase 26</t>
+  </si>
+  <si>
+    <t>Phase 27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -298,7 +350,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -575,21 +627,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +649,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -605,7 +657,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -613,7 +665,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -621,7 +673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -632,7 +684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -640,7 +692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -654,20 +706,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -678,7 +730,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
@@ -689,7 +741,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>38</v>
@@ -698,7 +750,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>39</v>
@@ -707,7 +759,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>40</v>
@@ -716,7 +768,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>41</v>
@@ -725,7 +777,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="1" t="s">
         <v>42</v>
@@ -734,7 +786,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="1" t="s">
         <v>43</v>
@@ -743,8 +795,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
       <c r="B9" s="1" t="s">
         <v>45</v>
       </c>
@@ -752,419 +804,821 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>31</v>
-      </c>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+      <c r="B13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="1" t="s">
+      <c r="C16" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="1" t="s">
+      <c r="C17" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="1" t="s">
+      <c r="C18" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="C19" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="5"/>
+      <c r="B27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="1" t="s">
+      <c r="C28" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="7"/>
+      <c r="B29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="1" t="s">
+      <c r="C29" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="7"/>
+      <c r="B30" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="1" t="s">
+      <c r="C30" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="7"/>
+      <c r="B31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="1" t="s">
+      <c r="C31" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="7"/>
+      <c r="B32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="1" t="s">
+      <c r="C32" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="1" t="s">
+      <c r="C33" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="1" t="s">
+      <c r="C34" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="1" t="s">
+      <c r="C35" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="1" t="s">
+      <c r="C36" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="C37" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="7"/>
+      <c r="B38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="7"/>
+      <c r="B41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="7"/>
+      <c r="B42" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="7"/>
+      <c r="B43" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="7"/>
+      <c r="B44" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="7"/>
+      <c r="B45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C45" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="7"/>
+      <c r="B46" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C46" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="7"/>
+      <c r="B47" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="7"/>
+      <c r="B48" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="7"/>
+      <c r="B49" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C49" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="7"/>
+      <c r="B50" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="7"/>
+      <c r="B51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="7"/>
+      <c r="B52" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="7"/>
+      <c r="B53" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="8"/>
+      <c r="B54" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B55" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="1" t="s">
+      <c r="C55" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="4"/>
+      <c r="B56" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4"/>
-      <c r="B28" s="1" t="s">
+      <c r="C56" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="4"/>
+      <c r="B57" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="1" t="s">
+      <c r="C57" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="4"/>
+      <c r="B58" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="1" t="s">
+      <c r="C58" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="4"/>
+      <c r="B59" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="1" t="s">
+      <c r="C59" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" s="4"/>
+      <c r="B60" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="1" t="s">
+      <c r="C60" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" s="4"/>
+      <c r="B61" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="C61" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" s="4"/>
+      <c r="B62" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C62" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="5"/>
+      <c r="B63" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="1" t="s">
+      <c r="C64" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="4"/>
+      <c r="B65" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="1" t="s">
+      <c r="C65" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="4"/>
+      <c r="B66" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="1" t="s">
+      <c r="C66" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="4"/>
+      <c r="B67" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="1" t="s">
+      <c r="C67" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="4"/>
+      <c r="B68" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="1" t="s">
+      <c r="C68" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" s="4"/>
+      <c r="B69" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="1" t="s">
+      <c r="C69" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" s="4"/>
+      <c r="B70" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="C70" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" s="4"/>
+      <c r="B71" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C71" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" s="4"/>
+      <c r="B72" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C72" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" s="4"/>
+      <c r="B73" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C73" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" s="4"/>
+      <c r="B74" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C74" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" s="4"/>
+      <c r="B75" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C75" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" s="4"/>
+      <c r="B76" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C76" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" s="4"/>
+      <c r="B77" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C77" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" s="4"/>
+      <c r="B78" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C78" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" s="4"/>
+      <c r="B79" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C79" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" s="4"/>
+      <c r="B80" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C80" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" s="5"/>
+      <c r="B81" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C81" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="1" t="s">
+      <c r="C82" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" s="4"/>
+      <c r="B83" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="1" t="s">
+      <c r="C83" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" s="4"/>
+      <c r="B84" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="1" t="s">
+      <c r="C84" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" s="4"/>
+      <c r="B85" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="1" t="s">
+      <c r="C85" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" s="4"/>
+      <c r="B86" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="1" t="s">
+      <c r="C86" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" s="4"/>
+      <c r="B87" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="1" t="s">
+      <c r="C87" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" s="4"/>
+      <c r="B88" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="1" t="s">
+      <c r="C88" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="4"/>
+      <c r="B89" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="1" t="s">
+      <c r="C89" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="4"/>
+      <c r="B90" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="5"/>
-      <c r="B49" s="1" t="s">
+      <c r="C90" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" s="5"/>
+      <c r="B91" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="C91" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B92" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="1" t="s">
+      <c r="C92" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" s="4"/>
+      <c r="B93" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="1" t="s">
+      <c r="C93" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" s="4"/>
+      <c r="B94" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="C94" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" s="4"/>
+      <c r="B95" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C95" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" s="5"/>
+      <c r="B96" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C96" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="1">
-        <f>SUM(C2:C52)</f>
-        <v>4800</v>
+      <c r="B97" s="2"/>
+      <c r="C97" s="1">
+        <f>SUM(C2:C96)</f>
+        <v>9500</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="A16:A25"/>
-    <mergeCell ref="A26:A32"/>
-    <mergeCell ref="A33:A39"/>
-    <mergeCell ref="A40:A49"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A82:A91"/>
+    <mergeCell ref="A92:A96"/>
+    <mergeCell ref="A55:A63"/>
+    <mergeCell ref="A28:A54"/>
+    <mergeCell ref="A64:A81"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A14:A27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1172,22 +1626,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B11" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1201,7 +1655,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -1213,7 +1667,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
@@ -1221,7 +1675,7 @@
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
@@ -1229,7 +1683,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>22</v>
@@ -1239,7 +1693,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="1" t="s">
@@ -1247,7 +1701,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="1" t="s">
@@ -1255,7 +1709,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>23</v>
@@ -1265,7 +1719,7 @@
       </c>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="1" t="s">
@@ -1273,7 +1727,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="1" t="s">
@@ -1281,7 +1735,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
         <v>24</v>
@@ -1291,7 +1745,7 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1" t="s">
@@ -1299,7 +1753,7 @@
       </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
@@ -1307,7 +1761,7 @@
       </c>
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1319,7 +1773,7 @@
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="9"/>
       <c r="C15" s="1" t="s">
@@ -1327,7 +1781,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="9"/>
       <c r="C16" s="1" t="s">
@@ -1335,7 +1789,7 @@
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>22</v>
@@ -1345,7 +1799,7 @@
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1" t="s">
@@ -1353,7 +1807,7 @@
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1" t="s">
@@ -1361,7 +1815,7 @@
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
         <v>23</v>
@@ -1371,7 +1825,7 @@
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="1" t="s">
@@ -1379,7 +1833,7 @@
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1" t="s">
@@ -1387,7 +1841,7 @@
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
         <v>24</v>
@@ -1397,7 +1851,7 @@
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="1" t="s">
@@ -1405,7 +1859,7 @@
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="1" t="s">
@@ -1413,7 +1867,7 @@
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
@@ -1425,7 +1879,7 @@
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="9"/>
       <c r="C27" s="1" t="s">
@@ -1433,7 +1887,7 @@
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="9"/>
       <c r="C28" s="1" t="s">
@@ -1441,7 +1895,7 @@
       </c>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
         <v>22</v>
@@ -1451,7 +1905,7 @@
       </c>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="1" t="s">
@@ -1459,7 +1913,7 @@
       </c>
       <c r="D30" s="1"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="1" t="s">
@@ -1467,7 +1921,7 @@
       </c>
       <c r="D31" s="1"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
         <v>23</v>
@@ -1477,7 +1931,7 @@
       </c>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="1" t="s">
@@ -1485,7 +1939,7 @@
       </c>
       <c r="D33" s="1"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="1" t="s">
@@ -1493,7 +1947,7 @@
       </c>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
         <v>24</v>
@@ -1503,7 +1957,7 @@
       </c>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="1" t="s">
@@ -1511,7 +1965,7 @@
       </c>
       <c r="D36" s="1"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="1" t="s">
@@ -1519,7 +1973,7 @@
       </c>
       <c r="D37" s="1"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>16</v>
       </c>
@@ -1531,7 +1985,7 @@
       </c>
       <c r="D38" s="1"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="9"/>
       <c r="C39" s="1" t="s">
@@ -1539,7 +1993,7 @@
       </c>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="9"/>
       <c r="C40" s="1" t="s">
@@ -1547,7 +2001,7 @@
       </c>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
         <v>22</v>
@@ -1557,7 +2011,7 @@
       </c>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="1" t="s">
@@ -1565,7 +2019,7 @@
       </c>
       <c r="D42" s="1"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="1" t="s">
@@ -1573,7 +2027,7 @@
       </c>
       <c r="D43" s="1"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
         <v>23</v>
@@ -1583,7 +2037,7 @@
       </c>
       <c r="D44" s="1"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="1" t="s">
@@ -1591,7 +2045,7 @@
       </c>
       <c r="D45" s="1"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="1" t="s">
@@ -1599,7 +2053,7 @@
       </c>
       <c r="D46" s="1"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
         <v>24</v>
@@ -1609,7 +2063,7 @@
       </c>
       <c r="D47" s="1"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="1" t="s">
@@ -1617,7 +2071,7 @@
       </c>
       <c r="D48" s="1"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="1" t="s">
@@ -1625,7 +2079,7 @@
       </c>
       <c r="D49" s="1"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>17</v>
       </c>
@@ -1637,7 +2091,7 @@
       </c>
       <c r="D50" s="1"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="1" t="s">
@@ -1645,7 +2099,7 @@
       </c>
       <c r="D51" s="1"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="1" t="s">
@@ -1653,7 +2107,7 @@
       </c>
       <c r="D52" s="1"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" s="9" t="s">
         <v>21</v>
@@ -1663,7 +2117,7 @@
       </c>
       <c r="D53" s="1"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" s="9"/>
       <c r="C54" s="1" t="s">
@@ -1671,7 +2125,7 @@
       </c>
       <c r="D54" s="1"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" s="9"/>
       <c r="C55" s="1" t="s">
@@ -1679,7 +2133,7 @@
       </c>
       <c r="D55" s="1"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
         <v>22</v>
@@ -1689,7 +2143,7 @@
       </c>
       <c r="D56" s="1"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="1" t="s">
@@ -1697,7 +2151,7 @@
       </c>
       <c r="D57" s="1"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="1" t="s">
@@ -1705,7 +2159,7 @@
       </c>
       <c r="D58" s="1"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="2" t="s">
         <v>23</v>
@@ -1715,7 +2169,7 @@
       </c>
       <c r="D59" s="1"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="1" t="s">
@@ -1723,7 +2177,7 @@
       </c>
       <c r="D60" s="1"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="1" t="s">
@@ -1731,7 +2185,7 @@
       </c>
       <c r="D61" s="1"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
         <v>24</v>
@@ -1741,7 +2195,7 @@
       </c>
       <c r="D62" s="1"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="1" t="s">
@@ -1749,7 +2203,7 @@
       </c>
       <c r="D63" s="1"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="1" t="s">

</xml_diff>

<commit_message>
update dataset spec - 06272020
</commit_message>
<xml_diff>
--- a/carla_dataset_spec.xlsx
+++ b/carla_dataset_spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Projects\TRIP_endtoend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6EF763-1147-45A9-A77D-AB42A776F868}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3A11C2-1A04-4A82-BF9A-7AAB5E627EAF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -250,16 +250,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,7 +622,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -642,10 +642,10 @@
       <c r="C1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="6"/>
+      <c r="G1" s="8"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -677,7 +677,7 @@
         <f t="shared" si="0"/>
         <v>1400</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="8" t="s">
         <v>41</v>
       </c>
       <c r="F3" s="1">
@@ -698,44 +698,60 @@
         <f t="shared" si="0"/>
         <v>3200</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="9">
-        <f>B9 * (F3/100)</f>
-        <v>99.84</v>
-      </c>
-      <c r="G4" s="9">
-        <f>B9 * (G3/100)</f>
-        <v>56.16</v>
+      <c r="E4" s="8"/>
+      <c r="F4" s="1">
+        <v>80</v>
+      </c>
+      <c r="G4" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>3100</v>
+        <v>3200</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="7">
+        <f>B9 * (F3/100)</f>
+        <v>122.88</v>
+      </c>
+      <c r="G5" s="7">
+        <f>B9 * (G3/100)</f>
+        <v>69.12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="1">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>1800</v>
+        <v>3400</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7">
+        <f>B9 * (F4/100)</f>
+        <v>153.60000000000002</v>
+      </c>
+      <c r="G6" s="7">
+        <f>B9 * (G4/100)</f>
+        <v>38.400000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="1">
@@ -747,15 +763,15 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="1">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>3400</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -764,19 +780,77 @@
       </c>
       <c r="B9" s="1">
         <f>SUM(B2:B8)</f>
-        <v>156</v>
+        <v>192</v>
       </c>
       <c r="C9" s="1">
         <f>SUM(C2:C8)</f>
-        <v>15600</v>
+        <v>19200</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="F1:G1"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="F3:G3">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{F942AF49-2BF7-43D4-B6C4-F3921954D388}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:G4">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0C809B68-E9A6-44A2-9A1B-142B297C066B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{F942AF49-2BF7-43D4-B6C4-F3921954D388}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F3:G3</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0C809B68-E9A6-44A2-9A1B-142B297C066B}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F4:G4</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -811,10 +885,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -823,24 +897,24 @@
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -849,24 +923,24 @@
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
       <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -875,24 +949,24 @@
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -901,26 +975,26 @@
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -929,24 +1003,24 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -955,24 +1029,24 @@
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -981,24 +1055,24 @@
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -1007,26 +1081,26 @@
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1035,24 +1109,24 @@
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
       <c r="C28" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D28" s="1"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6" t="s">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -1061,24 +1135,24 @@
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6" t="s">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1087,24 +1161,24 @@
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6" t="s">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1113,26 +1187,26 @@
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6"/>
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D37" s="1"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1141,24 +1215,24 @@
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="6"/>
-      <c r="B39" s="7"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="9"/>
       <c r="C39" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="6"/>
-      <c r="B40" s="7"/>
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6" t="s">
+      <c r="A41" s="8"/>
+      <c r="B41" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1167,24 +1241,24 @@
       <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
+      <c r="A42" s="8"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6" t="s">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1193,24 +1267,24 @@
       <c r="D44" s="1"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="6"/>
-      <c r="B45" s="6"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
       <c r="C45" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="6"/>
-      <c r="B46" s="6"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
       <c r="C46" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6" t="s">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -1219,26 +1293,26 @@
       <c r="D47" s="1"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
       <c r="C48" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D48" s="1"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
       <c r="C49" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -1247,24 +1321,24 @@
       <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6"/>
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
       <c r="C51" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
       <c r="C52" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="6"/>
-      <c r="B53" s="7" t="s">
+      <c r="A53" s="8"/>
+      <c r="B53" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C53" s="1" t="s">
@@ -1273,24 +1347,24 @@
       <c r="D53" s="1"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="6"/>
-      <c r="B54" s="7"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="9"/>
       <c r="C54" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D54" s="1"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="6"/>
-      <c r="B55" s="7"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="9"/>
       <c r="C55" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D55" s="1"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6" t="s">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -1299,24 +1373,24 @@
       <c r="D56" s="1"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="6"/>
-      <c r="B57" s="6"/>
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
       <c r="C57" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D57" s="1"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
       <c r="C58" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="6"/>
-      <c r="B59" s="6" t="s">
+      <c r="A59" s="8"/>
+      <c r="B59" s="8" t="s">
         <v>23</v>
       </c>
       <c r="C59" s="1" t="s">
@@ -1325,24 +1399,24 @@
       <c r="D59" s="1"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="6"/>
-      <c r="B60" s="6"/>
+      <c r="A60" s="8"/>
+      <c r="B60" s="8"/>
       <c r="C60" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D60" s="1"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="6"/>
-      <c r="B61" s="6"/>
+      <c r="A61" s="8"/>
+      <c r="B61" s="8"/>
       <c r="C61" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D61" s="1"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6" t="s">
+      <c r="A62" s="8"/>
+      <c r="B62" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C62" s="1" t="s">
@@ -1351,16 +1425,16 @@
       <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="6"/>
-      <c r="B63" s="6"/>
+      <c r="A63" s="8"/>
+      <c r="B63" s="8"/>
       <c r="C63" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D63" s="1"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="6"/>
-      <c r="B64" s="6"/>
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
       <c r="C64" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Update carla dataset spec file. Update copyfiles.py - 07/02/2020
</commit_message>
<xml_diff>
--- a/carla_dataset_spec.xlsx
+++ b/carla_dataset_spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Projects\TRIP_endtoend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3A11C2-1A04-4A82-BF9A-7AAB5E627EAF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BEAC35-B3FC-4717-98C3-469705623CEB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -622,7 +622,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -652,11 +652,11 @@
         <v>29</v>
       </c>
       <c r="B2" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1">
         <f t="shared" ref="C2:C8" si="0" xml:space="preserve"> B2 * 100</f>
-        <v>1100</v>
+        <v>1200</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="4" t="s">
@@ -667,15 +667,15 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="1">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" si="0"/>
-        <v>1400</v>
+        <v>3900</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>41</v>
@@ -722,11 +722,11 @@
       </c>
       <c r="F5" s="7">
         <f>B9 * (F3/100)</f>
-        <v>122.88</v>
+        <v>139.52000000000001</v>
       </c>
       <c r="G5" s="7">
         <f>B9 * (G3/100)</f>
-        <v>69.12</v>
+        <v>78.48</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -743,11 +743,11 @@
       <c r="E6" s="8"/>
       <c r="F6" s="7">
         <f>B9 * (F4/100)</f>
-        <v>153.60000000000002</v>
+        <v>174.4</v>
       </c>
       <c r="G6" s="7">
         <f>B9 * (G4/100)</f>
-        <v>38.400000000000006</v>
+        <v>43.6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -780,11 +780,11 @@
       </c>
       <c r="B9" s="1">
         <f>SUM(B2:B8)</f>
-        <v>192</v>
+        <v>218</v>
       </c>
       <c r="C9" s="1">
         <f>SUM(C2:C8)</f>
-        <v>19200</v>
+        <v>21800</v>
       </c>
     </row>
   </sheetData>
@@ -1442,11 +1442,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="B62:B64"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="A50:A64"/>
     <mergeCell ref="B35:B37"/>
@@ -1463,11 +1463,11 @@
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update dataset spec file - 07212020
</commit_message>
<xml_diff>
--- a/carla_dataset_spec.xlsx
+++ b/carla_dataset_spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Projects\TRIP_endtoend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13BEAC35-B3FC-4717-98C3-469705623CEB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC97E5E-74F4-4E40-BCCF-CF8AB024C357}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="12600" windowHeight="10404" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specifications" sheetId="1" r:id="rId1"/>
@@ -622,7 +622,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,7 +655,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="1">
-        <f t="shared" ref="C2:C8" si="0" xml:space="preserve"> B2 * 100</f>
+        <f xml:space="preserve"> B2 * 100</f>
         <v>1200</v>
       </c>
       <c r="E2" s="1"/>
@@ -674,7 +674,7 @@
         <v>39</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C2:C8" si="0" xml:space="preserve"> B3 * 100</f>
         <v>3900</v>
       </c>
       <c r="E3" s="8" t="s">
@@ -1442,11 +1442,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A38:A49"/>
     <mergeCell ref="A50:A64"/>
     <mergeCell ref="B35:B37"/>
@@ -1463,11 +1463,11 @@
     <mergeCell ref="B29:B31"/>
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="B62:B64"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>